<commit_message>
statistics of the day
</commit_message>
<xml_diff>
--- a/adm/12_Jan_09_31_Grades-5100-B1-2E16;Programmering_og_problemløsning.xlsx
+++ b/adm/12_Jan_09_31_Grades-5100-B1-2E16;Programmering_og_problemløsning.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27526"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27907"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sporring/repositories/PoP/adm/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="20" yWindow="0" windowWidth="25360" windowHeight="15220" tabRatio="500"/>
+    <workbookView xWindow="26980" yWindow="7200" windowWidth="25360" windowHeight="15220" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -13,8 +18,11 @@
     <definedName name="_12_Jan_09_31_Grades_5100_B1_2E16_Programmering_og_problemløsning" localSheetId="0">Sheet1!#REF!</definedName>
     <definedName name="_12_Jan_09_31_Grades_5100_B1_2E16_Programmering_og_problemløsning_1" localSheetId="0">Sheet1!$A$1:$R$233</definedName>
   </definedNames>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -25,7 +33,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="12_Jan_09_31_Grades-5100-B1-2E16;Programmering_og_problemløsning.csv" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="Macintosh HD:Users:sporring:Downloads:12_Jan_09_31_Grades-5100-B1-2E16;Programmering_og_problemløsning.csv" comma="1">
+    <textPr fileType="mac" sourceFile="Macintosh HD:Users:sporring:Downloads:12_Jan_09_31_Grades-5100-B1-2E16;Programmering_og_problemløsning.csv" comma="1">
       <textFields count="42">
         <textField type="text"/>
         <textField type="text"/>
@@ -3052,6 +3060,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -3297,11 +3310,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2110212232"/>
-        <c:axId val="2145078232"/>
+        <c:axId val="-1690991680"/>
+        <c:axId val="-1690989360"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2110212232"/>
+        <c:axId val="-1690991680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3311,7 +3324,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2145078232"/>
+        <c:crossAx val="-1690989360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3319,7 +3332,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2145078232"/>
+        <c:axId val="-1690989360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3330,7 +3343,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2110212232"/>
+        <c:crossAx val="-1690991680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3483,20 +3496,21 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2143988216"/>
-        <c:axId val="-2129544280"/>
+        <c:axId val="-1692588000"/>
+        <c:axId val="-1692716480"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2143988216"/>
+        <c:axId val="-1692588000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2129544280"/>
+        <c:crossAx val="-1692716480"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3504,7 +3518,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2129544280"/>
+        <c:axId val="-1692716480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3515,7 +3529,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2143988216"/>
+        <c:crossAx val="-1692588000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3930,11 +3944,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R247"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="G102" sqref="G102"/>
+    <sheetView tabSelected="1" topLeftCell="A228" workbookViewId="0">
+      <selection activeCell="A235" sqref="A235"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="33.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.33203125" bestFit="1" customWidth="1"/>
@@ -3954,7 +3968,7 @@
     <col min="18" max="18" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4008,12 +4022,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
       <c r="F2">
-        <f>SUM(G2:R2)</f>
+        <f t="shared" ref="F2:F65" si="0">SUM(G2:R2)</f>
         <v>12</v>
       </c>
       <c r="G2">
@@ -4053,7 +4067,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>77</v>
       </c>
@@ -4070,14 +4084,14 @@
         <v>542</v>
       </c>
       <c r="F3">
-        <f>SUM(G3:R3)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>138</v>
       </c>
@@ -4094,11 +4108,11 @@
         <v>49</v>
       </c>
       <c r="F4">
-        <f>SUM(G4:R4)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>158</v>
       </c>
@@ -4115,14 +4129,14 @@
         <v>624</v>
       </c>
       <c r="F5">
-        <f>SUM(G5:R5)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="P5">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>192</v>
       </c>
@@ -4139,14 +4153,14 @@
         <v>20</v>
       </c>
       <c r="F6">
-        <f>SUM(G6:R6)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G6">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:18">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>276</v>
       </c>
@@ -4163,11 +4177,11 @@
         <v>501</v>
       </c>
       <c r="F7">
-        <f>SUM(G7:R7)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>286</v>
       </c>
@@ -4184,11 +4198,11 @@
         <v>20</v>
       </c>
       <c r="F8">
-        <f>SUM(G8:R8)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>336</v>
       </c>
@@ -4205,11 +4219,11 @@
         <v>20</v>
       </c>
       <c r="F9">
-        <f>SUM(G9:R9)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>398</v>
       </c>
@@ -4226,14 +4240,14 @@
         <v>624</v>
       </c>
       <c r="F10">
-        <f>SUM(G10:R10)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="P10">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:18">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>418</v>
       </c>
@@ -4250,14 +4264,14 @@
         <v>613</v>
       </c>
       <c r="F11">
-        <f>SUM(G11:R11)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G11">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:18">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>426</v>
       </c>
@@ -4274,11 +4288,11 @@
         <v>49</v>
       </c>
       <c r="F12">
-        <f>SUM(G12:R12)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>452</v>
       </c>
@@ -4295,11 +4309,11 @@
         <v>501</v>
       </c>
       <c r="F13">
-        <f>SUM(G13:R13)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>472</v>
       </c>
@@ -4316,14 +4330,14 @@
         <v>28</v>
       </c>
       <c r="F14">
-        <f>SUM(G14:R14)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K14">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:18">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>186</v>
       </c>
@@ -4340,14 +4354,14 @@
         <v>653</v>
       </c>
       <c r="F15">
-        <f>SUM(G15:R15)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="G15">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:18">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>210</v>
       </c>
@@ -4364,14 +4378,14 @@
         <v>542</v>
       </c>
       <c r="F16">
-        <f>SUM(G16:R16)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="G16">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:16">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>222</v>
       </c>
@@ -4388,14 +4402,14 @@
         <v>23</v>
       </c>
       <c r="F17">
-        <f>SUM(G17:R17)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="G17">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:16">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>246</v>
       </c>
@@ -4412,14 +4426,14 @@
         <v>56</v>
       </c>
       <c r="F18">
-        <f>SUM(G18:R18)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="G18">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:16">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>290</v>
       </c>
@@ -4436,7 +4450,7 @@
         <v>501</v>
       </c>
       <c r="F19">
-        <f>SUM(G19:R19)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="G19">
@@ -4449,7 +4463,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:16">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>362</v>
       </c>
@@ -4466,14 +4480,14 @@
         <v>613</v>
       </c>
       <c r="F20">
-        <f>SUM(G20:R20)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="G20">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:16">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>69</v>
       </c>
@@ -4490,7 +4504,7 @@
         <v>23</v>
       </c>
       <c r="F21">
-        <f>SUM(G21:R21)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="G21">
@@ -4503,7 +4517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:16">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>216</v>
       </c>
@@ -4520,7 +4534,7 @@
         <v>542</v>
       </c>
       <c r="F22">
-        <f>SUM(G22:R22)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="G22">
@@ -4530,7 +4544,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:16">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>256</v>
       </c>
@@ -4547,7 +4561,7 @@
         <v>99</v>
       </c>
       <c r="F23">
-        <f>SUM(G23:R23)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="G23">
@@ -4557,7 +4571,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:16">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>296</v>
       </c>
@@ -4574,7 +4588,7 @@
         <v>23</v>
       </c>
       <c r="F24">
-        <f>SUM(G24:R24)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="H24">
@@ -4590,7 +4604,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:16">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
@@ -4607,7 +4621,7 @@
         <v>494</v>
       </c>
       <c r="F25">
-        <f>SUM(G25:R25)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="G25">
@@ -4620,7 +4634,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:16">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>32</v>
       </c>
@@ -4637,7 +4651,7 @@
         <v>501</v>
       </c>
       <c r="F26">
-        <f>SUM(G26:R26)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="G26">
@@ -4650,7 +4664,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:16">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>178</v>
       </c>
@@ -4667,7 +4681,7 @@
         <v>43</v>
       </c>
       <c r="F27">
-        <f>SUM(G27:R27)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="G27">
@@ -4680,7 +4694,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:16">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>320</v>
       </c>
@@ -4697,7 +4711,7 @@
         <v>43</v>
       </c>
       <c r="F28">
-        <f>SUM(G28:R28)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="G28">
@@ -4710,7 +4724,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:16">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>75</v>
       </c>
@@ -4727,7 +4741,7 @@
         <v>28</v>
       </c>
       <c r="F29">
-        <f>SUM(G29:R29)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="G29">
@@ -4749,7 +4763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:16">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>208</v>
       </c>
@@ -4766,7 +4780,7 @@
         <v>99</v>
       </c>
       <c r="F30">
-        <f>SUM(G30:R30)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="G30">
@@ -4788,7 +4802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:16">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>262</v>
       </c>
@@ -4805,7 +4819,7 @@
         <v>624</v>
       </c>
       <c r="F31">
-        <f>SUM(G31:R31)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="G31">
@@ -4833,7 +4847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:16">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>326</v>
       </c>
@@ -4850,7 +4864,7 @@
         <v>795</v>
       </c>
       <c r="F32">
-        <f>SUM(G32:R32)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="G32">
@@ -4872,7 +4886,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:16">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>91</v>
       </c>
@@ -4889,7 +4903,7 @@
         <v>23</v>
       </c>
       <c r="F33">
-        <f>SUM(G33:R33)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="G33">
@@ -4911,7 +4925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:16">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>206</v>
       </c>
@@ -4928,7 +4942,7 @@
         <v>674</v>
       </c>
       <c r="F34">
-        <f>SUM(G34:R34)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="G34">
@@ -4950,7 +4964,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:16">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>294</v>
       </c>
@@ -4967,7 +4981,7 @@
         <v>28</v>
       </c>
       <c r="F35">
-        <f>SUM(G35:R35)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="G35">
@@ -4989,7 +5003,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:16">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>146</v>
       </c>
@@ -5006,7 +5020,7 @@
         <v>99</v>
       </c>
       <c r="F36">
-        <f>SUM(G36:R36)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="G36">
@@ -5034,7 +5048,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:16">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>148</v>
       </c>
@@ -5051,7 +5065,7 @@
         <v>613</v>
       </c>
       <c r="F37">
-        <f>SUM(G37:R37)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="G37">
@@ -5076,7 +5090,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:16">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>288</v>
       </c>
@@ -5093,7 +5107,7 @@
         <v>674</v>
       </c>
       <c r="F38">
-        <f>SUM(G38:R38)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="G38">
@@ -5118,7 +5132,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:16">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>406</v>
       </c>
@@ -5135,7 +5149,7 @@
         <v>876</v>
       </c>
       <c r="F39">
-        <f>SUM(G39:R39)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="G39">
@@ -5160,7 +5174,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:16">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>57</v>
       </c>
@@ -5177,7 +5191,7 @@
         <v>28</v>
       </c>
       <c r="F40">
-        <f>SUM(G40:R40)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="G40">
@@ -5208,7 +5222,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:16">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>124</v>
       </c>
@@ -5225,7 +5239,7 @@
         <v>99</v>
       </c>
       <c r="F41">
-        <f>SUM(G41:R41)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="G41">
@@ -5259,7 +5273,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:16">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>166</v>
       </c>
@@ -5276,7 +5290,7 @@
         <v>56</v>
       </c>
       <c r="F42">
-        <f>SUM(G42:R42)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="G42">
@@ -5307,7 +5321,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:16">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>172</v>
       </c>
@@ -5324,7 +5338,7 @@
         <v>20</v>
       </c>
       <c r="F43">
-        <f>SUM(G43:R43)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="G43">
@@ -5355,7 +5369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:16">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>308</v>
       </c>
@@ -5372,7 +5386,7 @@
         <v>28</v>
       </c>
       <c r="F44">
-        <f>SUM(G44:R44)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="G44">
@@ -5406,7 +5420,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:16">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>332</v>
       </c>
@@ -5423,7 +5437,7 @@
         <v>20</v>
       </c>
       <c r="F45">
-        <f>SUM(G45:R45)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="G45">
@@ -5457,7 +5471,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:16">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>376</v>
       </c>
@@ -5474,7 +5488,7 @@
         <v>23</v>
       </c>
       <c r="F46">
-        <f>SUM(G46:R46)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="G46">
@@ -5502,7 +5516,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:16">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>390</v>
       </c>
@@ -5519,7 +5533,7 @@
         <v>494</v>
       </c>
       <c r="F47">
-        <f>SUM(G47:R47)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="G47">
@@ -5547,7 +5561,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:16">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>428</v>
       </c>
@@ -5564,7 +5578,7 @@
         <v>28</v>
       </c>
       <c r="F48">
-        <f>SUM(G48:R48)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="G48">
@@ -5592,7 +5606,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:16">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>478</v>
       </c>
@@ -5609,7 +5623,7 @@
         <v>46</v>
       </c>
       <c r="F49">
-        <f>SUM(G49:R49)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="G49">
@@ -5637,7 +5651,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:16">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>41</v>
       </c>
@@ -5654,7 +5668,7 @@
         <v>43</v>
       </c>
       <c r="F50">
-        <f>SUM(G50:R50)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="G50">
@@ -5682,7 +5696,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:16">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>67</v>
       </c>
@@ -5699,7 +5713,7 @@
         <v>28</v>
       </c>
       <c r="F51">
-        <f>SUM(G51:R51)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="G51">
@@ -5733,7 +5747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:16">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>73</v>
       </c>
@@ -5750,7 +5764,7 @@
         <v>28</v>
       </c>
       <c r="F52">
-        <f>SUM(G52:R52)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="G52">
@@ -5784,7 +5798,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:16">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>83</v>
       </c>
@@ -5801,7 +5815,7 @@
         <v>28</v>
       </c>
       <c r="F53">
-        <f>SUM(G53:R53)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="G53">
@@ -5835,7 +5849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:16">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>87</v>
       </c>
@@ -5852,7 +5866,7 @@
         <v>28</v>
       </c>
       <c r="F54">
-        <f>SUM(G54:R54)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="G54">
@@ -5886,7 +5900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:16">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>97</v>
       </c>
@@ -5903,7 +5917,7 @@
         <v>99</v>
       </c>
       <c r="F55">
-        <f>SUM(G55:R55)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="G55">
@@ -5937,7 +5951,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:16">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>132</v>
       </c>
@@ -5954,7 +5968,7 @@
         <v>49</v>
       </c>
       <c r="F56">
-        <f>SUM(G56:R56)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="G56">
@@ -5985,7 +5999,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:16">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>154</v>
       </c>
@@ -6002,7 +6016,7 @@
         <v>99</v>
       </c>
       <c r="F57">
-        <f>SUM(G57:R57)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="G57">
@@ -6036,7 +6050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:16">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>176</v>
       </c>
@@ -6053,7 +6067,7 @@
         <v>99</v>
       </c>
       <c r="F58">
-        <f>SUM(G58:R58)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="G58">
@@ -6087,7 +6101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:16">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>198</v>
       </c>
@@ -6104,7 +6118,7 @@
         <v>20</v>
       </c>
       <c r="F59">
-        <f>SUM(G59:R59)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="G59">
@@ -6138,7 +6152,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:16">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>218</v>
       </c>
@@ -6155,7 +6169,7 @@
         <v>49</v>
       </c>
       <c r="F60">
-        <f>SUM(G60:R60)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="G60">
@@ -6186,7 +6200,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:16">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>236</v>
       </c>
@@ -6203,7 +6217,7 @@
         <v>31</v>
       </c>
       <c r="F61">
-        <f>SUM(G61:R61)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="G61">
@@ -6237,7 +6251,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:16">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>238</v>
       </c>
@@ -6254,7 +6268,7 @@
         <v>46</v>
       </c>
       <c r="F62">
-        <f>SUM(G62:R62)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="G62">
@@ -6288,7 +6302,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:16">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>266</v>
       </c>
@@ -6305,7 +6319,7 @@
         <v>20</v>
       </c>
       <c r="F63">
-        <f>SUM(G63:R63)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="G63">
@@ -6339,7 +6353,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:16">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>292</v>
       </c>
@@ -6356,7 +6370,7 @@
         <v>99</v>
       </c>
       <c r="F64">
-        <f>SUM(G64:R64)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="G64">
@@ -6390,7 +6404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:16">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>302</v>
       </c>
@@ -6407,7 +6421,7 @@
         <v>99</v>
       </c>
       <c r="F65">
-        <f>SUM(G65:R65)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="G65">
@@ -6441,7 +6455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:16">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>304</v>
       </c>
@@ -6458,7 +6472,7 @@
         <v>99</v>
       </c>
       <c r="F66">
-        <f>SUM(G66:R66)</f>
+        <f t="shared" ref="F66:F129" si="1">SUM(G66:R66)</f>
         <v>8</v>
       </c>
       <c r="G66">
@@ -6492,7 +6506,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:16">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>340</v>
       </c>
@@ -6509,7 +6523,7 @@
         <v>23</v>
       </c>
       <c r="F67">
-        <f>SUM(G67:R67)</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="G67">
@@ -6540,7 +6554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:16">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>352</v>
       </c>
@@ -6557,7 +6571,7 @@
         <v>99</v>
       </c>
       <c r="F68">
-        <f>SUM(G68:R68)</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="G68">
@@ -6591,7 +6605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:16">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>360</v>
       </c>
@@ -6608,7 +6622,7 @@
         <v>99</v>
       </c>
       <c r="F69">
-        <f>SUM(G69:R69)</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="G69">
@@ -6642,7 +6656,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:16">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>364</v>
       </c>
@@ -6659,7 +6673,7 @@
         <v>28</v>
       </c>
       <c r="F70">
-        <f>SUM(G70:R70)</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="G70">
@@ -6693,7 +6707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:16">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>372</v>
       </c>
@@ -6710,7 +6724,7 @@
         <v>49</v>
       </c>
       <c r="F71">
-        <f>SUM(G71:R71)</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="G71">
@@ -6738,7 +6752,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:16">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>374</v>
       </c>
@@ -6755,7 +6769,7 @@
         <v>46</v>
       </c>
       <c r="F72">
-        <f>SUM(G72:R72)</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="G72">
@@ -6789,7 +6803,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:16">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>382</v>
       </c>
@@ -6806,7 +6820,7 @@
         <v>99</v>
       </c>
       <c r="F73">
-        <f>SUM(G73:R73)</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="G73">
@@ -6840,7 +6854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:16">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>396</v>
       </c>
@@ -6857,7 +6871,7 @@
         <v>99</v>
       </c>
       <c r="F74">
-        <f>SUM(G74:R74)</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="G74">
@@ -6891,7 +6905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:16">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>404</v>
       </c>
@@ -6908,7 +6922,7 @@
         <v>28</v>
       </c>
       <c r="F75">
-        <f>SUM(G75:R75)</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="G75">
@@ -6942,7 +6956,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:16">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>408</v>
       </c>
@@ -6959,7 +6973,7 @@
         <v>99</v>
       </c>
       <c r="F76">
-        <f>SUM(G76:R76)</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="G76">
@@ -6993,7 +7007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:16">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>414</v>
       </c>
@@ -7010,7 +7024,7 @@
         <v>28</v>
       </c>
       <c r="F77">
-        <f>SUM(G77:R77)</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="G77">
@@ -7044,7 +7058,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:16">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>434</v>
       </c>
@@ -7061,7 +7075,7 @@
         <v>99</v>
       </c>
       <c r="F78">
-        <f>SUM(G78:R78)</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="G78">
@@ -7095,7 +7109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:16">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>468</v>
       </c>
@@ -7112,7 +7126,7 @@
         <v>99</v>
       </c>
       <c r="F79">
-        <f>SUM(G79:R79)</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="G79">
@@ -7146,7 +7160,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:16">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>474</v>
       </c>
@@ -7163,7 +7177,7 @@
         <v>99</v>
       </c>
       <c r="F80">
-        <f>SUM(G80:R80)</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="G80">
@@ -7197,7 +7211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:16">
+    <row r="81" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>44</v>
       </c>
@@ -7214,7 +7228,7 @@
         <v>46</v>
       </c>
       <c r="F81">
-        <f>SUM(G81:R81)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="G81">
@@ -7248,7 +7262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:16">
+    <row r="82" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>50</v>
       </c>
@@ -7265,7 +7279,7 @@
         <v>23</v>
       </c>
       <c r="F82">
-        <f>SUM(G82:R82)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="G82">
@@ -7299,7 +7313,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:16">
+    <row r="83" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>59</v>
       </c>
@@ -7316,7 +7330,7 @@
         <v>20</v>
       </c>
       <c r="F83">
-        <f>SUM(G83:R83)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="G83">
@@ -7350,7 +7364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:16">
+    <row r="84" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>63</v>
       </c>
@@ -7367,7 +7381,7 @@
         <v>28</v>
       </c>
       <c r="F84">
-        <f>SUM(G84:R84)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="G84">
@@ -7401,7 +7415,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:16">
+    <row r="85" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>81</v>
       </c>
@@ -7418,7 +7432,7 @@
         <v>46</v>
       </c>
       <c r="F85">
-        <f>SUM(G85:R85)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="G85">
@@ -7452,7 +7466,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:16">
+    <row r="86" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>108</v>
       </c>
@@ -7469,7 +7483,7 @@
         <v>28</v>
       </c>
       <c r="F86">
-        <f>SUM(G86:R86)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="G86">
@@ -7503,7 +7517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:16">
+    <row r="87" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>114</v>
       </c>
@@ -7520,7 +7534,7 @@
         <v>20</v>
       </c>
       <c r="F87">
-        <f>SUM(G87:R87)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="G87">
@@ -7554,7 +7568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:16">
+    <row r="88" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>120</v>
       </c>
@@ -7571,7 +7585,7 @@
         <v>99</v>
       </c>
       <c r="F88">
-        <f>SUM(G88:R88)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="G88">
@@ -7605,7 +7619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:16">
+    <row r="89" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>122</v>
       </c>
@@ -7622,7 +7636,7 @@
         <v>23</v>
       </c>
       <c r="F89">
-        <f>SUM(G89:R89)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="G89">
@@ -7656,7 +7670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:16">
+    <row r="90" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>134</v>
       </c>
@@ -7673,7 +7687,7 @@
         <v>20</v>
       </c>
       <c r="F90">
-        <f>SUM(G90:R90)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="G90">
@@ -7707,7 +7721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:16">
+    <row r="91" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
         <v>142</v>
       </c>
@@ -7724,7 +7738,7 @@
         <v>20</v>
       </c>
       <c r="F91">
-        <f>SUM(G91:R91)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="G91">
@@ -7758,7 +7772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:16">
+    <row r="92" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
         <v>150</v>
       </c>
@@ -7775,7 +7789,7 @@
         <v>28</v>
       </c>
       <c r="F92">
-        <f>SUM(G92:R92)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="G92">
@@ -7809,7 +7823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:16">
+    <row r="93" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
         <v>156</v>
       </c>
@@ -7826,7 +7840,7 @@
         <v>43</v>
       </c>
       <c r="F93">
-        <f>SUM(G93:R93)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="G93">
@@ -7860,7 +7874,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:16">
+    <row r="94" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>162</v>
       </c>
@@ -7877,7 +7891,7 @@
         <v>56</v>
       </c>
       <c r="F94">
-        <f>SUM(G94:R94)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="G94">
@@ -7911,7 +7925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:16">
+    <row r="95" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>168</v>
       </c>
@@ -7928,7 +7942,7 @@
         <v>23</v>
       </c>
       <c r="F95">
-        <f>SUM(G95:R95)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="G95">
@@ -7962,7 +7976,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:16">
+    <row r="96" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
         <v>188</v>
       </c>
@@ -7979,7 +7993,7 @@
         <v>28</v>
       </c>
       <c r="F96">
-        <f>SUM(G96:R96)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="G96">
@@ -8013,7 +8027,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:16">
+    <row r="97" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
         <v>190</v>
       </c>
@@ -8030,7 +8044,7 @@
         <v>43</v>
       </c>
       <c r="F97">
-        <f>SUM(G97:R97)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="G97">
@@ -8064,7 +8078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:16">
+    <row r="98" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
         <v>194</v>
       </c>
@@ -8081,7 +8095,7 @@
         <v>28</v>
       </c>
       <c r="F98">
-        <f>SUM(G98:R98)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="G98">
@@ -8115,7 +8129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:16">
+    <row r="99" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
         <v>196</v>
       </c>
@@ -8132,7 +8146,7 @@
         <v>31</v>
       </c>
       <c r="F99">
-        <f>SUM(G99:R99)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="G99">
@@ -8166,7 +8180,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:16">
+    <row r="100" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
         <v>200</v>
       </c>
@@ -8183,7 +8197,7 @@
         <v>23</v>
       </c>
       <c r="F100">
-        <f>SUM(G100:R100)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="G100">
@@ -8217,7 +8231,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:16">
+    <row r="101" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
         <v>202</v>
       </c>
@@ -8234,7 +8248,7 @@
         <v>31</v>
       </c>
       <c r="F101">
-        <f>SUM(G101:R101)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="G101">
@@ -8268,7 +8282,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:16">
+    <row r="102" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
         <v>214</v>
       </c>
@@ -8285,7 +8299,7 @@
         <v>20</v>
       </c>
       <c r="F102">
-        <f>SUM(G102:R102)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="G102">
@@ -8319,7 +8333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:16">
+    <row r="103" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
         <v>224</v>
       </c>
@@ -8336,7 +8350,7 @@
         <v>46</v>
       </c>
       <c r="F103">
-        <f>SUM(G103:R103)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="G103">
@@ -8370,7 +8384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:16">
+    <row r="104" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
         <v>226</v>
       </c>
@@ -8387,7 +8401,7 @@
         <v>23</v>
       </c>
       <c r="F104">
-        <f>SUM(G104:R104)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="G104">
@@ -8421,7 +8435,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:16">
+    <row r="105" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
         <v>230</v>
       </c>
@@ -8438,7 +8452,7 @@
         <v>28</v>
       </c>
       <c r="F105">
-        <f>SUM(G105:R105)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="G105">
@@ -8472,7 +8486,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:16">
+    <row r="106" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
         <v>232</v>
       </c>
@@ -8489,7 +8503,7 @@
         <v>23</v>
       </c>
       <c r="F106">
-        <f>SUM(G106:R106)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="G106">
@@ -8520,7 +8534,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:16">
+    <row r="107" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
         <v>244</v>
       </c>
@@ -8537,7 +8551,7 @@
         <v>20</v>
       </c>
       <c r="F107">
-        <f>SUM(G107:R107)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="G107">
@@ -8571,7 +8585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:16">
+    <row r="108" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
         <v>258</v>
       </c>
@@ -8588,7 +8602,7 @@
         <v>23</v>
       </c>
       <c r="F108">
-        <f>SUM(G108:R108)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="G108">
@@ -8622,7 +8636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:16">
+    <row r="109" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
         <v>268</v>
       </c>
@@ -8639,7 +8653,7 @@
         <v>46</v>
       </c>
       <c r="F109">
-        <f>SUM(G109:R109)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="G109">
@@ -8673,7 +8687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:16">
+    <row r="110" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
         <v>270</v>
       </c>
@@ -8690,7 +8704,7 @@
         <v>46</v>
       </c>
       <c r="F110">
-        <f>SUM(G110:R110)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="G110">
@@ -8724,7 +8738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:16">
+    <row r="111" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
         <v>272</v>
       </c>
@@ -8741,7 +8755,7 @@
         <v>20</v>
       </c>
       <c r="F111">
-        <f>SUM(G111:R111)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="G111">
@@ -8775,7 +8789,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:16">
+    <row r="112" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
         <v>278</v>
       </c>
@@ -8792,7 +8806,7 @@
         <v>20</v>
       </c>
       <c r="F112">
-        <f>SUM(G112:R112)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="G112">
@@ -8826,7 +8840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:16">
+    <row r="113" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
         <v>280</v>
       </c>
@@ -8843,7 +8857,7 @@
         <v>56</v>
       </c>
       <c r="F113">
-        <f>SUM(G113:R113)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="G113">
@@ -8877,7 +8891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:16">
+    <row r="114" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
         <v>282</v>
       </c>
@@ -8894,7 +8908,7 @@
         <v>46</v>
       </c>
       <c r="F114">
-        <f>SUM(G114:R114)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="G114">
@@ -8928,7 +8942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:16">
+    <row r="115" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
         <v>298</v>
       </c>
@@ -8945,7 +8959,7 @@
         <v>23</v>
       </c>
       <c r="F115">
-        <f>SUM(G115:R115)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="G115">
@@ -8979,7 +8993,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:16">
+    <row r="116" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
         <v>314</v>
       </c>
@@ -8996,7 +9010,7 @@
         <v>46</v>
       </c>
       <c r="F116">
-        <f>SUM(G116:R116)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="G116">
@@ -9030,7 +9044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:16">
+    <row r="117" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
         <v>316</v>
       </c>
@@ -9047,7 +9061,7 @@
         <v>28</v>
       </c>
       <c r="F117">
-        <f>SUM(G117:R117)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="G117">
@@ -9081,7 +9095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:16">
+    <row r="118" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
         <v>318</v>
       </c>
@@ -9098,7 +9112,7 @@
         <v>56</v>
       </c>
       <c r="F118">
-        <f>SUM(G118:R118)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="G118">
@@ -9132,7 +9146,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:16">
+    <row r="119" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
         <v>330</v>
       </c>
@@ -9149,7 +9163,7 @@
         <v>28</v>
       </c>
       <c r="F119">
-        <f>SUM(G119:R119)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="G119">
@@ -9183,7 +9197,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:16">
+    <row r="120" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
         <v>342</v>
       </c>
@@ -9200,7 +9214,7 @@
         <v>99</v>
       </c>
       <c r="F120">
-        <f>SUM(G120:R120)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="G120">
@@ -9234,7 +9248,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:16">
+    <row r="121" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
         <v>346</v>
       </c>
@@ -9251,7 +9265,7 @@
         <v>43</v>
       </c>
       <c r="F121">
-        <f>SUM(G121:R121)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="G121">
@@ -9285,7 +9299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:16">
+    <row r="122" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
         <v>348</v>
       </c>
@@ -9302,7 +9316,7 @@
         <v>46</v>
       </c>
       <c r="F122">
-        <f>SUM(G122:R122)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="G122">
@@ -9336,7 +9350,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:16">
+    <row r="123" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
         <v>354</v>
       </c>
@@ -9353,7 +9367,7 @@
         <v>46</v>
       </c>
       <c r="F123">
-        <f>SUM(G123:R123)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="G123">
@@ -9387,7 +9401,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:16">
+    <row r="124" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
         <v>366</v>
       </c>
@@ -9404,7 +9418,7 @@
         <v>28</v>
       </c>
       <c r="F124">
-        <f>SUM(G124:R124)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="G124">
@@ -9438,7 +9452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:16">
+    <row r="125" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
         <v>380</v>
       </c>
@@ -9455,7 +9469,7 @@
         <v>46</v>
       </c>
       <c r="F125">
-        <f>SUM(G125:R125)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="G125">
@@ -9489,7 +9503,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:16">
+    <row r="126" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
         <v>384</v>
       </c>
@@ -9506,7 +9520,7 @@
         <v>31</v>
       </c>
       <c r="F126">
-        <f>SUM(G126:R126)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="G126">
@@ -9540,7 +9554,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:16">
+    <row r="127" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
         <v>402</v>
       </c>
@@ -9557,7 +9571,7 @@
         <v>43</v>
       </c>
       <c r="F127">
-        <f>SUM(G127:R127)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="G127">
@@ -9591,7 +9605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:16">
+    <row r="128" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
         <v>410</v>
       </c>
@@ -9608,7 +9622,7 @@
         <v>43</v>
       </c>
       <c r="F128">
-        <f>SUM(G128:R128)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="G128">
@@ -9639,7 +9653,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:16">
+    <row r="129" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
         <v>440</v>
       </c>
@@ -9656,7 +9670,7 @@
         <v>20</v>
       </c>
       <c r="F129">
-        <f>SUM(G129:R129)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="G129">
@@ -9690,7 +9704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:16">
+    <row r="130" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
         <v>442</v>
       </c>
@@ -9707,7 +9721,7 @@
         <v>23</v>
       </c>
       <c r="F130">
-        <f>SUM(G130:R130)</f>
+        <f t="shared" ref="F130:F193" si="2">SUM(G130:R130)</f>
         <v>9</v>
       </c>
       <c r="G130">
@@ -9741,7 +9755,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:16">
+    <row r="131" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
         <v>446</v>
       </c>
@@ -9758,7 +9772,7 @@
         <v>49</v>
       </c>
       <c r="F131">
-        <f>SUM(G131:R131)</f>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="G131">
@@ -9792,7 +9806,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:16">
+    <row r="132" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
         <v>448</v>
       </c>
@@ -9809,7 +9823,7 @@
         <v>49</v>
       </c>
       <c r="F132">
-        <f>SUM(G132:R132)</f>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="G132">
@@ -9843,7 +9857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:16">
+    <row r="133" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
         <v>450</v>
       </c>
@@ -9860,7 +9874,7 @@
         <v>46</v>
       </c>
       <c r="F133">
-        <f>SUM(G133:R133)</f>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="G133">
@@ -9894,7 +9908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:16">
+    <row r="134" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
         <v>456</v>
       </c>
@@ -9911,7 +9925,7 @@
         <v>46</v>
       </c>
       <c r="F134">
-        <f>SUM(G134:R134)</f>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="G134">
@@ -9945,7 +9959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:16">
+    <row r="135" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
         <v>462</v>
       </c>
@@ -9962,7 +9976,7 @@
         <v>28</v>
       </c>
       <c r="F135">
-        <f>SUM(G135:R135)</f>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="G135">
@@ -9996,7 +10010,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:16">
+    <row r="136" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
         <v>482</v>
       </c>
@@ -10013,7 +10027,7 @@
         <v>20</v>
       </c>
       <c r="F136">
-        <f>SUM(G136:R136)</f>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="G136">
@@ -10047,7 +10061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:16">
+    <row r="137" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
         <v>484</v>
       </c>
@@ -10064,7 +10078,7 @@
         <v>49</v>
       </c>
       <c r="F137">
-        <f>SUM(G137:R137)</f>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="G137">
@@ -10098,7 +10112,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:16">
+    <row r="138" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
         <v>18</v>
       </c>
@@ -10115,7 +10129,7 @@
         <v>20</v>
       </c>
       <c r="F138">
-        <f>SUM(G138:R138)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="G138">
@@ -10149,7 +10163,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:16">
+    <row r="139" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
         <v>21</v>
       </c>
@@ -10166,7 +10180,7 @@
         <v>23</v>
       </c>
       <c r="F139">
-        <f>SUM(G139:R139)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="G139">
@@ -10200,7 +10214,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:16">
+    <row r="140" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
         <v>26</v>
       </c>
@@ -10217,7 +10231,7 @@
         <v>28</v>
       </c>
       <c r="F140">
-        <f>SUM(G140:R140)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="G140">
@@ -10251,7 +10265,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:16">
+    <row r="141" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
         <v>29</v>
       </c>
@@ -10268,7 +10282,7 @@
         <v>31</v>
       </c>
       <c r="F141">
-        <f>SUM(G141:R141)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="G141">
@@ -10302,7 +10316,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:16">
+    <row r="142" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
         <v>34</v>
       </c>
@@ -10319,7 +10333,7 @@
         <v>31</v>
       </c>
       <c r="F142">
-        <f>SUM(G142:R142)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="G142">
@@ -10353,7 +10367,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:16">
+    <row r="143" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
         <v>36</v>
       </c>
@@ -10370,7 +10384,7 @@
         <v>38</v>
       </c>
       <c r="F143">
-        <f>SUM(G143:R143)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="G143">
@@ -10404,7 +10418,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:16">
+    <row r="144" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
         <v>39</v>
       </c>
@@ -10421,7 +10435,7 @@
         <v>31</v>
       </c>
       <c r="F144">
-        <f>SUM(G144:R144)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="G144">
@@ -10455,7 +10469,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:16">
+    <row r="145" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
         <v>47</v>
       </c>
@@ -10472,7 +10486,7 @@
         <v>49</v>
       </c>
       <c r="F145">
-        <f>SUM(G145:R145)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="G145">
@@ -10506,7 +10520,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:16">
+    <row r="146" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
         <v>52</v>
       </c>
@@ -10523,7 +10537,7 @@
         <v>31</v>
       </c>
       <c r="F146">
-        <f>SUM(G146:R146)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="G146">
@@ -10557,7 +10571,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:16">
+    <row r="147" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
         <v>54</v>
       </c>
@@ -10574,7 +10588,7 @@
         <v>56</v>
       </c>
       <c r="F147">
-        <f>SUM(G147:R147)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="G147">
@@ -10608,7 +10622,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:16">
+    <row r="148" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
         <v>61</v>
       </c>
@@ -10625,7 +10639,7 @@
         <v>31</v>
       </c>
       <c r="F148">
-        <f>SUM(G148:R148)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="G148">
@@ -10659,7 +10673,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:16">
+    <row r="149" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
         <v>65</v>
       </c>
@@ -10676,7 +10690,7 @@
         <v>49</v>
       </c>
       <c r="F149">
-        <f>SUM(G149:R149)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="G149">
@@ -10710,7 +10724,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="1:16">
+    <row r="150" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
         <v>71</v>
       </c>
@@ -10727,7 +10741,7 @@
         <v>43</v>
       </c>
       <c r="F150">
-        <f>SUM(G150:R150)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="G150">
@@ -10761,7 +10775,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:16">
+    <row r="151" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
         <v>79</v>
       </c>
@@ -10778,7 +10792,7 @@
         <v>49</v>
       </c>
       <c r="F151">
-        <f>SUM(G151:R151)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="G151">
@@ -10812,7 +10826,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="1:16">
+    <row r="152" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
         <v>85</v>
       </c>
@@ -10829,7 +10843,7 @@
         <v>46</v>
       </c>
       <c r="F152">
-        <f>SUM(G152:R152)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="G152">
@@ -10863,7 +10877,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="1:16">
+    <row r="153" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
         <v>89</v>
       </c>
@@ -10880,7 +10894,7 @@
         <v>49</v>
       </c>
       <c r="F153">
-        <f>SUM(G153:R153)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="G153">
@@ -10914,7 +10928,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="154" spans="1:16">
+    <row r="154" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="s">
         <v>93</v>
       </c>
@@ -10931,7 +10945,7 @@
         <v>31</v>
       </c>
       <c r="F154">
-        <f>SUM(G154:R154)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="G154">
@@ -10965,7 +10979,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="1:16">
+    <row r="155" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="s">
         <v>95</v>
       </c>
@@ -10982,7 +10996,7 @@
         <v>28</v>
       </c>
       <c r="F155">
-        <f>SUM(G155:R155)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="G155">
@@ -11016,7 +11030,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="156" spans="1:16">
+    <row r="156" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A156" s="1" t="s">
         <v>100</v>
       </c>
@@ -11033,7 +11047,7 @@
         <v>49</v>
       </c>
       <c r="F156">
-        <f>SUM(G156:R156)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="G156">
@@ -11067,7 +11081,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="1:16">
+    <row r="157" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A157" s="1" t="s">
         <v>102</v>
       </c>
@@ -11084,7 +11098,7 @@
         <v>23</v>
       </c>
       <c r="F157">
-        <f>SUM(G157:R157)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="G157">
@@ -11118,7 +11132,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="1:16">
+    <row r="158" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A158" s="1" t="s">
         <v>104</v>
       </c>
@@ -11135,7 +11149,7 @@
         <v>23</v>
       </c>
       <c r="F158">
-        <f>SUM(G158:R158)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="G158">
@@ -11169,7 +11183,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="159" spans="1:16">
+    <row r="159" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A159" s="1" t="s">
         <v>106</v>
       </c>
@@ -11186,7 +11200,7 @@
         <v>20</v>
       </c>
       <c r="F159">
-        <f>SUM(G159:R159)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="G159">
@@ -11220,7 +11234,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="160" spans="1:16">
+    <row r="160" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A160" s="1" t="s">
         <v>110</v>
       </c>
@@ -11237,7 +11251,7 @@
         <v>56</v>
       </c>
       <c r="F160">
-        <f>SUM(G160:R160)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="G160">
@@ -11271,7 +11285,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="1:16">
+    <row r="161" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A161" s="1" t="s">
         <v>112</v>
       </c>
@@ -11288,7 +11302,7 @@
         <v>31</v>
       </c>
       <c r="F161">
-        <f>SUM(G161:R161)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="G161">
@@ -11322,7 +11336,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="1:16">
+    <row r="162" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A162" s="1" t="s">
         <v>116</v>
       </c>
@@ -11339,7 +11353,7 @@
         <v>23</v>
       </c>
       <c r="F162">
-        <f>SUM(G162:R162)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="G162">
@@ -11373,7 +11387,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="163" spans="1:16">
+    <row r="163" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A163" s="1" t="s">
         <v>118</v>
       </c>
@@ -11390,7 +11404,7 @@
         <v>23</v>
       </c>
       <c r="F163">
-        <f>SUM(G163:R163)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="G163">
@@ -11424,7 +11438,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="164" spans="1:16">
+    <row r="164" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A164" s="1" t="s">
         <v>126</v>
       </c>
@@ -11441,7 +11455,7 @@
         <v>31</v>
       </c>
       <c r="F164">
-        <f>SUM(G164:R164)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="G164">
@@ -11475,7 +11489,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="165" spans="1:16">
+    <row r="165" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A165" s="1" t="s">
         <v>128</v>
       </c>
@@ -11492,7 +11506,7 @@
         <v>23</v>
       </c>
       <c r="F165">
-        <f>SUM(G165:R165)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="G165">
@@ -11526,7 +11540,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="166" spans="1:16">
+    <row r="166" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A166" s="1" t="s">
         <v>130</v>
       </c>
@@ -11543,7 +11557,7 @@
         <v>56</v>
       </c>
       <c r="F166">
-        <f>SUM(G166:R166)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="G166">
@@ -11577,7 +11591,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="167" spans="1:16">
+    <row r="167" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A167" s="1" t="s">
         <v>136</v>
       </c>
@@ -11594,7 +11608,7 @@
         <v>43</v>
       </c>
       <c r="F167">
-        <f>SUM(G167:R167)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="G167">
@@ -11628,7 +11642,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="168" spans="1:16">
+    <row r="168" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A168" s="1" t="s">
         <v>140</v>
       </c>
@@ -11645,7 +11659,7 @@
         <v>56</v>
       </c>
       <c r="F168">
-        <f>SUM(G168:R168)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="G168">
@@ -11679,7 +11693,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="169" spans="1:16">
+    <row r="169" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A169" s="1" t="s">
         <v>144</v>
       </c>
@@ -11696,7 +11710,7 @@
         <v>23</v>
       </c>
       <c r="F169">
-        <f>SUM(G169:R169)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="G169">
@@ -11730,7 +11744,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="170" spans="1:16">
+    <row r="170" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A170" s="1" t="s">
         <v>152</v>
       </c>
@@ -11747,7 +11761,7 @@
         <v>56</v>
       </c>
       <c r="F170">
-        <f>SUM(G170:R170)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="G170">
@@ -11781,7 +11795,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="171" spans="1:16">
+    <row r="171" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A171" s="1" t="s">
         <v>160</v>
       </c>
@@ -11798,7 +11812,7 @@
         <v>28</v>
       </c>
       <c r="F171">
-        <f>SUM(G171:R171)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="G171">
@@ -11832,7 +11846,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="172" spans="1:16">
+    <row r="172" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A172" s="1" t="s">
         <v>164</v>
       </c>
@@ -11849,7 +11863,7 @@
         <v>31</v>
       </c>
       <c r="F172">
-        <f>SUM(G172:R172)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="G172">
@@ -11883,7 +11897,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="173" spans="1:16">
+    <row r="173" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A173" s="1" t="s">
         <v>170</v>
       </c>
@@ -11900,7 +11914,7 @@
         <v>56</v>
       </c>
       <c r="F173">
-        <f>SUM(G173:R173)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="G173">
@@ -11934,7 +11948,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="174" spans="1:16">
+    <row r="174" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A174" s="1" t="s">
         <v>174</v>
       </c>
@@ -11951,7 +11965,7 @@
         <v>49</v>
       </c>
       <c r="F174">
-        <f>SUM(G174:R174)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="G174">
@@ -11985,7 +11999,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="175" spans="1:16">
+    <row r="175" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A175" s="1" t="s">
         <v>180</v>
       </c>
@@ -12002,7 +12016,7 @@
         <v>23</v>
       </c>
       <c r="F175">
-        <f>SUM(G175:R175)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="G175">
@@ -12036,7 +12050,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="176" spans="1:16">
+    <row r="176" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A176" s="1" t="s">
         <v>182</v>
       </c>
@@ -12053,7 +12067,7 @@
         <v>23</v>
       </c>
       <c r="F176">
-        <f>SUM(G176:R176)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="G176">
@@ -12087,7 +12101,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="177" spans="1:16">
+    <row r="177" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A177" s="1" t="s">
         <v>184</v>
       </c>
@@ -12104,7 +12118,7 @@
         <v>49</v>
       </c>
       <c r="F177">
-        <f>SUM(G177:R177)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="G177">
@@ -12138,7 +12152,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="178" spans="1:16">
+    <row r="178" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A178" s="1" t="s">
         <v>204</v>
       </c>
@@ -12155,7 +12169,7 @@
         <v>31</v>
       </c>
       <c r="F178">
-        <f>SUM(G178:R178)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="G178">
@@ -12189,7 +12203,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="179" spans="1:16">
+    <row r="179" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A179" s="1" t="s">
         <v>212</v>
       </c>
@@ -12206,7 +12220,7 @@
         <v>28</v>
       </c>
       <c r="F179">
-        <f>SUM(G179:R179)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="G179">
@@ -12240,7 +12254,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="180" spans="1:16">
+    <row r="180" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A180" s="1" t="s">
         <v>220</v>
       </c>
@@ -12257,7 +12271,7 @@
         <v>46</v>
       </c>
       <c r="F180">
-        <f>SUM(G180:R180)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="G180">
@@ -12291,7 +12305,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="181" spans="1:16">
+    <row r="181" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A181" s="1" t="s">
         <v>228</v>
       </c>
@@ -12308,7 +12322,7 @@
         <v>56</v>
       </c>
       <c r="F181">
-        <f>SUM(G181:R181)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="G181">
@@ -12342,7 +12356,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="182" spans="1:16">
+    <row r="182" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A182" s="1" t="s">
         <v>234</v>
       </c>
@@ -12359,7 +12373,7 @@
         <v>28</v>
       </c>
       <c r="F182">
-        <f>SUM(G182:R182)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="G182">
@@ -12393,7 +12407,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="183" spans="1:16">
+    <row r="183" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A183" s="1" t="s">
         <v>240</v>
       </c>
@@ -12410,7 +12424,7 @@
         <v>31</v>
       </c>
       <c r="F183">
-        <f>SUM(G183:R183)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="G183">
@@ -12444,7 +12458,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="184" spans="1:16">
+    <row r="184" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A184" s="1" t="s">
         <v>242</v>
       </c>
@@ -12461,7 +12475,7 @@
         <v>28</v>
       </c>
       <c r="F184">
-        <f>SUM(G184:R184)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="G184">
@@ -12495,7 +12509,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="185" spans="1:16">
+    <row r="185" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A185" s="1" t="s">
         <v>248</v>
       </c>
@@ -12512,7 +12526,7 @@
         <v>31</v>
       </c>
       <c r="F185">
-        <f>SUM(G185:R185)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="G185">
@@ -12546,7 +12560,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="186" spans="1:16">
+    <row r="186" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A186" s="1" t="s">
         <v>250</v>
       </c>
@@ -12563,7 +12577,7 @@
         <v>38</v>
       </c>
       <c r="F186">
-        <f>SUM(G186:R186)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="G186">
@@ -12597,7 +12611,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="187" spans="1:16">
+    <row r="187" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A187" s="1" t="s">
         <v>252</v>
       </c>
@@ -12614,7 +12628,7 @@
         <v>43</v>
       </c>
       <c r="F187">
-        <f>SUM(G187:R187)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="G187">
@@ -12648,7 +12662,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="188" spans="1:16">
+    <row r="188" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A188" s="1" t="s">
         <v>254</v>
       </c>
@@ -12665,7 +12679,7 @@
         <v>49</v>
       </c>
       <c r="F188">
-        <f>SUM(G188:R188)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="G188">
@@ -12699,7 +12713,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="189" spans="1:16">
+    <row r="189" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A189" s="1" t="s">
         <v>260</v>
       </c>
@@ -12716,7 +12730,7 @@
         <v>31</v>
       </c>
       <c r="F189">
-        <f>SUM(G189:R189)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="G189">
@@ -12750,7 +12764,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="190" spans="1:16">
+    <row r="190" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A190" s="1" t="s">
         <v>264</v>
       </c>
@@ -12767,7 +12781,7 @@
         <v>20</v>
       </c>
       <c r="F190">
-        <f>SUM(G190:R190)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="G190">
@@ -12801,7 +12815,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="191" spans="1:16">
+    <row r="191" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A191" s="1" t="s">
         <v>274</v>
       </c>
@@ -12818,7 +12832,7 @@
         <v>28</v>
       </c>
       <c r="F191">
-        <f>SUM(G191:R191)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="G191">
@@ -12852,7 +12866,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="192" spans="1:16">
+    <row r="192" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A192" s="1" t="s">
         <v>284</v>
       </c>
@@ -12869,7 +12883,7 @@
         <v>56</v>
       </c>
       <c r="F192">
-        <f>SUM(G192:R192)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="G192">
@@ -12903,7 +12917,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="193" spans="1:16">
+    <row r="193" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A193" s="1" t="s">
         <v>300</v>
       </c>
@@ -12920,7 +12934,7 @@
         <v>31</v>
       </c>
       <c r="F193">
-        <f>SUM(G193:R193)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="G193">
@@ -12954,7 +12968,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="194" spans="1:16">
+    <row r="194" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A194" s="1" t="s">
         <v>306</v>
       </c>
@@ -12971,7 +12985,7 @@
         <v>46</v>
       </c>
       <c r="F194">
-        <f>SUM(G194:R194)</f>
+        <f t="shared" ref="F194:F257" si="3">SUM(G194:R194)</f>
         <v>10</v>
       </c>
       <c r="G194">
@@ -13005,7 +13019,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="195" spans="1:16">
+    <row r="195" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A195" s="1" t="s">
         <v>310</v>
       </c>
@@ -13022,7 +13036,7 @@
         <v>46</v>
       </c>
       <c r="F195">
-        <f>SUM(G195:R195)</f>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="G195">
@@ -13056,7 +13070,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="196" spans="1:16">
+    <row r="196" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A196" s="1" t="s">
         <v>312</v>
       </c>
@@ -13073,7 +13087,7 @@
         <v>43</v>
       </c>
       <c r="F196">
-        <f>SUM(G196:R196)</f>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="G196">
@@ -13107,7 +13121,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="197" spans="1:16">
+    <row r="197" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A197" s="1" t="s">
         <v>322</v>
       </c>
@@ -13124,7 +13138,7 @@
         <v>46</v>
       </c>
       <c r="F197">
-        <f>SUM(G197:R197)</f>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="G197">
@@ -13158,7 +13172,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="198" spans="1:16">
+    <row r="198" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A198" s="1" t="s">
         <v>324</v>
       </c>
@@ -13175,7 +13189,7 @@
         <v>46</v>
       </c>
       <c r="F198">
-        <f>SUM(G198:R198)</f>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="G198">
@@ -13209,7 +13223,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="199" spans="1:16">
+    <row r="199" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A199" s="1" t="s">
         <v>328</v>
       </c>
@@ -13226,7 +13240,7 @@
         <v>28</v>
       </c>
       <c r="F199">
-        <f>SUM(G199:R199)</f>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="G199">
@@ -13260,7 +13274,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="200" spans="1:16">
+    <row r="200" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A200" s="1" t="s">
         <v>334</v>
       </c>
@@ -13277,7 +13291,7 @@
         <v>46</v>
       </c>
       <c r="F200">
-        <f>SUM(G200:R200)</f>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="G200">
@@ -13311,7 +13325,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="201" spans="1:16">
+    <row r="201" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A201" s="1" t="s">
         <v>338</v>
       </c>
@@ -13328,7 +13342,7 @@
         <v>23</v>
       </c>
       <c r="F201">
-        <f>SUM(G201:R201)</f>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="G201">
@@ -13362,7 +13376,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="202" spans="1:16">
+    <row r="202" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A202" s="1" t="s">
         <v>344</v>
       </c>
@@ -13379,7 +13393,7 @@
         <v>43</v>
       </c>
       <c r="F202">
-        <f>SUM(G202:R202)</f>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="G202">
@@ -13413,7 +13427,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="203" spans="1:16">
+    <row r="203" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A203" s="1" t="s">
         <v>350</v>
       </c>
@@ -13430,7 +13444,7 @@
         <v>56</v>
       </c>
       <c r="F203">
-        <f>SUM(G203:R203)</f>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="G203">
@@ -13464,7 +13478,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="204" spans="1:16">
+    <row r="204" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A204" s="1" t="s">
         <v>356</v>
       </c>
@@ -13481,7 +13495,7 @@
         <v>43</v>
       </c>
       <c r="F204">
-        <f>SUM(G204:R204)</f>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="G204">
@@ -13515,7 +13529,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="205" spans="1:16">
+    <row r="205" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A205" s="1" t="s">
         <v>358</v>
       </c>
@@ -13532,7 +13546,7 @@
         <v>49</v>
       </c>
       <c r="F205">
-        <f>SUM(G205:R205)</f>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="G205">
@@ -13566,7 +13580,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="206" spans="1:16">
+    <row r="206" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A206" s="1" t="s">
         <v>368</v>
       </c>
@@ -13583,7 +13597,7 @@
         <v>56</v>
       </c>
       <c r="F206">
-        <f>SUM(G206:R206)</f>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="G206">
@@ -13617,7 +13631,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="207" spans="1:16">
+    <row r="207" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A207" s="1" t="s">
         <v>370</v>
       </c>
@@ -13634,7 +13648,7 @@
         <v>49</v>
       </c>
       <c r="F207">
-        <f>SUM(G207:R207)</f>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="G207">
@@ -13668,7 +13682,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="208" spans="1:16">
+    <row r="208" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A208" s="1" t="s">
         <v>378</v>
       </c>
@@ -13685,7 +13699,7 @@
         <v>56</v>
       </c>
       <c r="F208">
-        <f>SUM(G208:R208)</f>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="G208">
@@ -13719,7 +13733,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="209" spans="1:16">
+    <row r="209" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A209" s="1" t="s">
         <v>386</v>
       </c>
@@ -13736,7 +13750,7 @@
         <v>23</v>
       </c>
       <c r="F209">
-        <f>SUM(G209:R209)</f>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="G209">
@@ -13770,7 +13784,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="210" spans="1:16">
+    <row r="210" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A210" s="1" t="s">
         <v>388</v>
       </c>
@@ -13787,7 +13801,7 @@
         <v>31</v>
       </c>
       <c r="F210">
-        <f>SUM(G210:R210)</f>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="G210">
@@ -13821,7 +13835,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="211" spans="1:16">
+    <row r="211" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A211" s="1" t="s">
         <v>392</v>
       </c>
@@ -13838,7 +13852,7 @@
         <v>23</v>
       </c>
       <c r="F211">
-        <f>SUM(G211:R211)</f>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="G211">
@@ -13872,7 +13886,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="212" spans="1:16">
+    <row r="212" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A212" s="1" t="s">
         <v>394</v>
       </c>
@@ -13889,7 +13903,7 @@
         <v>46</v>
       </c>
       <c r="F212">
-        <f>SUM(G212:R212)</f>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="G212">
@@ -13923,7 +13937,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="213" spans="1:16">
+    <row r="213" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A213" s="1" t="s">
         <v>400</v>
       </c>
@@ -13940,7 +13954,7 @@
         <v>20</v>
       </c>
       <c r="F213">
-        <f>SUM(G213:R213)</f>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="G213">
@@ -13974,7 +13988,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="214" spans="1:16">
+    <row r="214" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A214" s="1" t="s">
         <v>412</v>
       </c>
@@ -13991,7 +14005,7 @@
         <v>49</v>
       </c>
       <c r="F214">
-        <f>SUM(G214:R214)</f>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="G214">
@@ -14025,7 +14039,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="215" spans="1:16">
+    <row r="215" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A215" s="1" t="s">
         <v>416</v>
       </c>
@@ -14042,7 +14056,7 @@
         <v>31</v>
       </c>
       <c r="F215">
-        <f>SUM(G215:R215)</f>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="G215">
@@ -14076,7 +14090,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="216" spans="1:16">
+    <row r="216" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A216" s="1" t="s">
         <v>420</v>
       </c>
@@ -14093,7 +14107,7 @@
         <v>56</v>
       </c>
       <c r="F216">
-        <f>SUM(G216:R216)</f>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="G216">
@@ -14127,7 +14141,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="217" spans="1:16">
+    <row r="217" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A217" s="1" t="s">
         <v>422</v>
       </c>
@@ -14144,7 +14158,7 @@
         <v>56</v>
       </c>
       <c r="F217">
-        <f>SUM(G217:R217)</f>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="G217">
@@ -14178,7 +14192,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="218" spans="1:16">
+    <row r="218" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A218" s="1" t="s">
         <v>424</v>
       </c>
@@ -14195,7 +14209,7 @@
         <v>38</v>
       </c>
       <c r="F218">
-        <f>SUM(G218:R218)</f>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="G218">
@@ -14229,7 +14243,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="219" spans="1:16">
+    <row r="219" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A219" s="1" t="s">
         <v>430</v>
       </c>
@@ -14246,7 +14260,7 @@
         <v>23</v>
       </c>
       <c r="F219">
-        <f>SUM(G219:R219)</f>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="G219">
@@ -14280,7 +14294,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="220" spans="1:16">
+    <row r="220" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A220" s="1" t="s">
         <v>432</v>
       </c>
@@ -14297,7 +14311,7 @@
         <v>31</v>
       </c>
       <c r="F220">
-        <f>SUM(G220:R220)</f>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="G220">
@@ -14331,7 +14345,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="221" spans="1:16">
+    <row r="221" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A221" s="1" t="s">
         <v>436</v>
       </c>
@@ -14348,7 +14362,7 @@
         <v>20</v>
       </c>
       <c r="F221">
-        <f>SUM(G221:R221)</f>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="G221">
@@ -14382,7 +14396,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="222" spans="1:16">
+    <row r="222" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A222" s="1" t="s">
         <v>438</v>
       </c>
@@ -14399,7 +14413,7 @@
         <v>49</v>
       </c>
       <c r="F222">
-        <f>SUM(G222:R222)</f>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="G222">
@@ -14433,7 +14447,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="223" spans="1:16">
+    <row r="223" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A223" s="1" t="s">
         <v>444</v>
       </c>
@@ -14450,7 +14464,7 @@
         <v>56</v>
       </c>
       <c r="F223">
-        <f>SUM(G223:R223)</f>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="G223">
@@ -14484,7 +14498,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="224" spans="1:16">
+    <row r="224" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A224" s="1" t="s">
         <v>454</v>
       </c>
@@ -14501,7 +14515,7 @@
         <v>28</v>
       </c>
       <c r="F224">
-        <f>SUM(G224:R224)</f>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="G224">
@@ -14535,7 +14549,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="225" spans="1:18">
+    <row r="225" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A225" s="1" t="s">
         <v>458</v>
       </c>
@@ -14552,7 +14566,7 @@
         <v>23</v>
       </c>
       <c r="F225">
-        <f>SUM(G225:R225)</f>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="G225">
@@ -14586,7 +14600,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="226" spans="1:18">
+    <row r="226" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A226" s="1" t="s">
         <v>460</v>
       </c>
@@ -14603,7 +14617,7 @@
         <v>43</v>
       </c>
       <c r="F226">
-        <f>SUM(G226:R226)</f>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="G226">
@@ -14637,7 +14651,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="227" spans="1:18">
+    <row r="227" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A227" s="1" t="s">
         <v>464</v>
       </c>
@@ -14654,7 +14668,7 @@
         <v>28</v>
       </c>
       <c r="F227">
-        <f>SUM(G227:R227)</f>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="G227">
@@ -14688,7 +14702,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="228" spans="1:18">
+    <row r="228" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A228" s="1" t="s">
         <v>466</v>
       </c>
@@ -14705,7 +14719,7 @@
         <v>49</v>
       </c>
       <c r="F228">
-        <f>SUM(G228:R228)</f>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="G228">
@@ -14739,7 +14753,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="229" spans="1:18">
+    <row r="229" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A229" s="1" t="s">
         <v>470</v>
       </c>
@@ -14756,7 +14770,7 @@
         <v>56</v>
       </c>
       <c r="F229">
-        <f>SUM(G229:R229)</f>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="G229">
@@ -14790,7 +14804,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="230" spans="1:18">
+    <row r="230" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A230" s="1" t="s">
         <v>476</v>
       </c>
@@ -14807,7 +14821,7 @@
         <v>43</v>
       </c>
       <c r="F230">
-        <f>SUM(G230:R230)</f>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="G230">
@@ -14841,7 +14855,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="231" spans="1:18">
+    <row r="231" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A231" s="1" t="s">
         <v>480</v>
       </c>
@@ -14858,7 +14872,7 @@
         <v>43</v>
       </c>
       <c r="F231">
-        <f>SUM(G231:R231)</f>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="G231">
@@ -14892,7 +14906,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="232" spans="1:18">
+    <row r="232" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A232" s="1" t="s">
         <v>486</v>
       </c>
@@ -14909,7 +14923,7 @@
         <v>38</v>
       </c>
       <c r="F232">
-        <f>SUM(G232:R232)</f>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="G232">
@@ -14943,7 +14957,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="233" spans="1:18">
+    <row r="233" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A233" s="1"/>
       <c r="B233" s="1"/>
       <c r="D233" s="1"/>
@@ -14957,51 +14971,51 @@
         <v>217</v>
       </c>
       <c r="H233">
-        <f t="shared" ref="H233:R233" si="0">SUM(H3:H232)</f>
+        <f t="shared" ref="H233:R233" si="4">SUM(H3:H232)</f>
         <v>209</v>
       </c>
       <c r="I233">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>195</v>
       </c>
       <c r="J233">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>209</v>
       </c>
       <c r="K233">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>188</v>
       </c>
       <c r="L233">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>203</v>
       </c>
       <c r="M233">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>171</v>
       </c>
       <c r="N233">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>192</v>
       </c>
       <c r="O233">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>152</v>
       </c>
       <c r="P233">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>126</v>
       </c>
       <c r="Q233">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="R233">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="235" spans="1:18">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="235" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A235" s="1" t="s">
         <v>957</v>
       </c>
@@ -15012,7 +15026,7 @@
         <v>959</v>
       </c>
     </row>
-    <row r="236" spans="1:18">
+    <row r="236" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A236">
         <v>1</v>
       </c>
@@ -15025,7 +15039,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="237" spans="1:18">
+    <row r="237" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A237">
         <v>2</v>
       </c>
@@ -15038,7 +15052,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="238" spans="1:18">
+    <row r="238" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A238">
         <v>3</v>
       </c>
@@ -15047,11 +15061,11 @@
         <v>4</v>
       </c>
       <c r="C238">
-        <f t="shared" ref="C238:C247" si="1">C237+B238</f>
+        <f t="shared" ref="C238:C247" si="5">C237+B238</f>
         <v>14</v>
       </c>
     </row>
-    <row r="239" spans="1:18">
+    <row r="239" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A239">
         <v>4</v>
       </c>
@@ -15060,11 +15074,11 @@
         <v>4</v>
       </c>
       <c r="C239">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>18</v>
       </c>
     </row>
-    <row r="240" spans="1:18">
+    <row r="240" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A240">
         <v>5</v>
       </c>
@@ -15073,11 +15087,11 @@
         <v>3</v>
       </c>
       <c r="C240">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>21</v>
       </c>
     </row>
-    <row r="241" spans="1:3">
+    <row r="241" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A241">
         <v>6</v>
       </c>
@@ -15086,11 +15100,11 @@
         <v>4</v>
       </c>
       <c r="C241">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>25</v>
       </c>
     </row>
-    <row r="242" spans="1:3">
+    <row r="242" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A242">
         <v>7</v>
       </c>
@@ -15099,11 +15113,11 @@
         <v>10</v>
       </c>
       <c r="C242">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>35</v>
       </c>
     </row>
-    <row r="243" spans="1:3">
+    <row r="243" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A243">
         <v>8</v>
       </c>
@@ -15112,11 +15126,11 @@
         <v>31</v>
       </c>
       <c r="C243">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>66</v>
       </c>
     </row>
-    <row r="244" spans="1:3">
+    <row r="244" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A244">
         <v>9</v>
       </c>
@@ -15125,11 +15139,11 @@
         <v>57</v>
       </c>
       <c r="C244">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>123</v>
       </c>
     </row>
-    <row r="245" spans="1:3">
+    <row r="245" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A245">
         <v>10</v>
       </c>
@@ -15138,11 +15152,11 @@
         <v>95</v>
       </c>
       <c r="C245">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>218</v>
       </c>
     </row>
-    <row r="246" spans="1:3">
+    <row r="246" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A246">
         <v>11</v>
       </c>
@@ -15151,11 +15165,11 @@
         <v>0</v>
       </c>
       <c r="C246">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>218</v>
       </c>
     </row>
-    <row r="247" spans="1:3">
+    <row r="247" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A247">
         <v>12</v>
       </c>
@@ -15164,7 +15178,7 @@
         <v>0</v>
       </c>
       <c r="C247">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>218</v>
       </c>
     </row>
@@ -15175,10 +15189,5 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>